<commit_message>
Hice Imprimir Presupuesto y muchos cambios para que funcione
</commit_message>
<xml_diff>
--- a/Ventas.xlsx
+++ b/Ventas.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,6 +405,9 @@
       <c r="H1" t="str">
         <v>fecha</v>
       </c>
+      <c r="I1" t="str">
+        <v>cobrado</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -414,13 +417,13 @@
         <v>Presupuesto</v>
       </c>
       <c r="C2" t="str">
-        <v>0007-00000005</v>
+        <v>0002-00047601</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>124.38</v>
+        <v>506.46</v>
       </c>
       <c r="F2" t="str">
         <v>AGUSTIN</v>
@@ -429,12 +432,452 @@
         <v>Electro Avenida</v>
       </c>
       <c r="H2" t="str">
-        <v>23/04/2022</v>
+        <v>27/04/2022 - 8:6:0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>TISERA YANINA</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C3" t="str">
+        <v>0004-00019168</v>
+      </c>
+      <c r="E3">
+        <v>1592.1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="H3" t="str">
+        <v>27/04/2022 - 8:14:55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>LORENZATTO AGUSTIN</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Presupuesto</v>
+      </c>
+      <c r="C4" t="str">
+        <v>0002-00047603</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-506.46</v>
+      </c>
+      <c r="F4" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H4" t="str">
+        <v>27/04/2022 - 8:16:24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>COOP. DE TRABAJO HORIZONTE DE CHAJRI LTD</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Recibos</v>
+      </c>
+      <c r="C5" t="str">
+        <v>0004-00019169</v>
+      </c>
+      <c r="E5">
+        <v>23868.27</v>
+      </c>
+      <c r="F5" t="str">
+        <v>SILVIA</v>
+      </c>
+      <c r="H5" t="str">
+        <v>27/04/2022 - 9:7:24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>AGROPETROLERA CHAJARI S.R.L.</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C6" t="str">
+        <v>0004-00019170</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H6" t="str">
+        <v>27/04/2022 - 9:39:22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>AGROPETROLERA CHAJARI S.R.L.</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C7" t="str">
+        <v>0004-00019171</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H7" t="str">
+        <v>27/04/2022 - 9:40:22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>LA NUEVA S.R.L.</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Ticket Factura</v>
+      </c>
+      <c r="C8" t="str">
+        <v>0005-00000006</v>
+      </c>
+      <c r="D8">
+        <v>0.03</v>
+      </c>
+      <c r="E8">
+        <v>0.65</v>
+      </c>
+      <c r="F8" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H8" t="str">
+        <v>27/04/2022 - 9:47:59</v>
+      </c>
+      <c r="I8">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>Presupuesto</v>
+      </c>
+      <c r="C9" t="str">
+        <v>0002-00047604</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>18530.53</v>
+      </c>
+      <c r="F9" t="str">
+        <v>MARINA</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H9" t="str">
+        <v>27/04/2022 - 10:0:24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>ASOC. CIV.INSTITUTO C/REDENTOR</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C10" t="str">
+        <v>0004-00019172</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H10" t="str">
+        <v>27/04/2022 - 10:11:59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ASOCIACION REGIONAL DE TRANSPORTE</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C11" t="str">
+        <v>0004-00019173</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H11" t="str">
+        <v>27/04/2022 - 10:29:1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>MASETTO MARIA BELEN</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C12" t="str">
+        <v>0004-00019174</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <v>PABLO</v>
+      </c>
+      <c r="H12" t="str">
+        <v>27/04/2022 - 11:22:11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>A CONSUMIDOR FINAL</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Ticket Factura</v>
+      </c>
+      <c r="C13" t="str">
+        <v>0005-00000026</v>
+      </c>
+      <c r="D13">
+        <v>0.18</v>
+      </c>
+      <c r="E13">
+        <v>350</v>
+      </c>
+      <c r="F13" t="str">
+        <v>YANINA</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H13" t="str">
+        <v>27/04/2022 - 11:47:15</v>
+      </c>
+      <c r="I13">
+        <v>349.82</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>A CONSUMIDOR FINAL</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Ticket Factura</v>
+      </c>
+      <c r="C14" t="str">
+        <v>0005-00000027</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>380</v>
+      </c>
+      <c r="F14" t="str">
+        <v>PABLO</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H14" t="str">
+        <v>27/04/2022 - 11:49:35</v>
+      </c>
+      <c r="I14">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>LORENZATTO AGUSTIN</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Ticket Factura</v>
+      </c>
+      <c r="C15" t="str">
+        <v>0005-00000028</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.68</v>
+      </c>
+      <c r="F15" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H15" t="str">
+        <v>27/04/2022 - 11:50:33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>A CONSUMIDOR FINAL</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Ticket Factura</v>
+      </c>
+      <c r="C16" t="str">
+        <v>0005-00000029</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.48</v>
+      </c>
+      <c r="F16" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H16" t="str">
+        <v>27/04/2022 - 11:52:41</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>MUNICIPALIDAD DE CHAJARI</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C17" t="str">
+        <v>0004-00019176</v>
+      </c>
+      <c r="E17">
+        <v>172692</v>
+      </c>
+      <c r="F17" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H17" t="str">
+        <v>27/04/2022 - 12:7:55</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>MUNICIPALIDAD DE CHAJARI</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C18" t="str">
+        <v>0004-00019177</v>
+      </c>
+      <c r="E18">
+        <v>12450</v>
+      </c>
+      <c r="F18" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H18" t="str">
+        <v>27/04/2022 - 12:8:27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>MUNICIPALIDAD DE CHAJARI</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C19" t="str">
+        <v>0004-00019178</v>
+      </c>
+      <c r="E19">
+        <v>7146</v>
+      </c>
+      <c r="F19" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="H19" t="str">
+        <v>27/04/2022 - 12:9:45</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>A CONSUMIDOR FINAL</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Presupuesto</v>
+      </c>
+      <c r="C20" t="str">
+        <v>0002-00047605</v>
+      </c>
+      <c r="D20">
+        <v>-4.15</v>
+      </c>
+      <c r="E20">
+        <v>-2780</v>
+      </c>
+      <c r="F20" t="str">
+        <v>ELBIO</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Electro Avenida</v>
+      </c>
+      <c r="H20" t="str">
+        <v>27/04/2022 - 12:19:33</v>
+      </c>
+      <c r="I20">
+        <v>-2775.85</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>FABRELLO HERMANOS</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Recibos_P</v>
+      </c>
+      <c r="C21" t="str">
+        <v>0004-00019179</v>
+      </c>
+      <c r="E21">
+        <v>131370.1</v>
+      </c>
+      <c r="F21" t="str">
+        <v>AGUSTIN</v>
+      </c>
+      <c r="H21" t="str">
+        <v>27/04/2022 - 15:35:12</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>